<commit_message>
Adição de caso teste. Artigo. Pequenos recursos adicionais.
</commit_message>
<xml_diff>
--- a/material/casos.xlsx
+++ b/material/casos.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="rascunho" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>caso010</t>
   </si>
@@ -95,6 +95,18 @@
   <si>
     <t>Minas / Células livres</t>
   </si>
+  <si>
+    <t>pt1</t>
+  </si>
+  <si>
+    <t>pt2</t>
+  </si>
+  <si>
+    <t>Atual</t>
+  </si>
+  <si>
+    <t>delim</t>
+  </si>
 </sst>
 </file>
 
@@ -102,9 +114,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,8 +138,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +169,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -175,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -184,11 +228,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -10963,12 +11016,1107 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:AP36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26:Y36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="38" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="C2" s="10">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2</v>
+      </c>
+      <c r="E2" s="10">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10">
+        <v>4</v>
+      </c>
+      <c r="G2" s="10">
+        <v>5</v>
+      </c>
+      <c r="H2" s="10">
+        <v>6</v>
+      </c>
+      <c r="I2" s="10">
+        <v>7</v>
+      </c>
+      <c r="J2" s="10">
+        <v>8</v>
+      </c>
+      <c r="K2" s="10">
+        <v>9</v>
+      </c>
+      <c r="L2" s="10">
+        <v>10</v>
+      </c>
+      <c r="P2" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>2</v>
+      </c>
+      <c r="R2" s="10">
+        <v>3</v>
+      </c>
+      <c r="S2" s="10">
+        <v>4</v>
+      </c>
+      <c r="T2" s="10">
+        <v>5</v>
+      </c>
+      <c r="U2" s="10">
+        <v>6</v>
+      </c>
+      <c r="V2" s="10">
+        <v>7</v>
+      </c>
+      <c r="W2" s="10">
+        <v>8</v>
+      </c>
+      <c r="X2" s="10">
+        <v>9</v>
+      </c>
+      <c r="Y2" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="O3" s="10">
+        <v>1</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="AO3">
+        <v>3</v>
+      </c>
+      <c r="AP3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B4" s="10">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="O4" s="10">
+        <v>2</v>
+      </c>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="AO4">
+        <v>2</v>
+      </c>
+      <c r="AP4">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B5" s="10">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="O5" s="10">
+        <v>3</v>
+      </c>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="AO5">
+        <v>4</v>
+      </c>
+      <c r="AP5">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B6" s="10">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="O6" s="10">
+        <v>4</v>
+      </c>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+    </row>
+    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B7" s="10">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="O7" s="10">
+        <v>5</v>
+      </c>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+    </row>
+    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" s="10">
+        <v>6</v>
+      </c>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B9" s="10">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="O9" s="10">
+        <v>7</v>
+      </c>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+    </row>
+    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B10" s="10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="O10" s="10">
+        <v>8</v>
+      </c>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+    </row>
+    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="O11" s="10">
+        <v>9</v>
+      </c>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+    </row>
+    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="O12" s="10">
+        <v>10</v>
+      </c>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+    </row>
+    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="C14" s="10">
+        <v>1</v>
+      </c>
+      <c r="D14" s="10">
+        <v>2</v>
+      </c>
+      <c r="E14" s="10">
+        <v>3</v>
+      </c>
+      <c r="F14" s="10">
+        <v>4</v>
+      </c>
+      <c r="G14" s="10">
+        <v>5</v>
+      </c>
+      <c r="H14" s="10">
+        <v>6</v>
+      </c>
+      <c r="I14" s="10">
+        <v>7</v>
+      </c>
+      <c r="J14" s="10">
+        <v>8</v>
+      </c>
+      <c r="K14" s="10">
+        <v>9</v>
+      </c>
+      <c r="L14" s="10">
+        <v>10</v>
+      </c>
+      <c r="P14" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>2</v>
+      </c>
+      <c r="R14" s="10">
+        <v>3</v>
+      </c>
+      <c r="S14" s="10">
+        <v>4</v>
+      </c>
+      <c r="T14" s="10">
+        <v>5</v>
+      </c>
+      <c r="U14" s="10">
+        <v>6</v>
+      </c>
+      <c r="V14" s="10">
+        <v>7</v>
+      </c>
+      <c r="W14" s="10">
+        <v>8</v>
+      </c>
+      <c r="X14" s="10">
+        <v>9</v>
+      </c>
+      <c r="Y14" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B15" s="10">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="O15" s="10">
+        <v>1</v>
+      </c>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+    </row>
+    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="B16" s="10">
+        <v>2</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="O16" s="10">
+        <v>2</v>
+      </c>
+      <c r="P16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+    </row>
+    <row r="17" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B17" s="10">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="O17" s="10">
+        <v>3</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+    </row>
+    <row r="18" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B18" s="10">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="O18" s="10">
+        <v>4</v>
+      </c>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B19" s="10">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="O19" s="10">
+        <v>5</v>
+      </c>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B20" s="10">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="O20" s="10">
+        <v>6</v>
+      </c>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B21" s="10">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="O21" s="10">
+        <v>7</v>
+      </c>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+    </row>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B22" s="10">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="O22" s="10">
+        <v>8</v>
+      </c>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+    </row>
+    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B23" s="10">
+        <v>9</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="O23" s="10">
+        <v>9</v>
+      </c>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+    </row>
+    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B24" s="10">
+        <v>10</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="O24" s="10">
+        <v>10</v>
+      </c>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+    </row>
+    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C26" s="10">
+        <v>1</v>
+      </c>
+      <c r="D26" s="10">
+        <v>2</v>
+      </c>
+      <c r="E26" s="10">
+        <v>3</v>
+      </c>
+      <c r="F26" s="10">
+        <v>4</v>
+      </c>
+      <c r="G26" s="10">
+        <v>5</v>
+      </c>
+      <c r="H26" s="10">
+        <v>6</v>
+      </c>
+      <c r="I26" s="10">
+        <v>7</v>
+      </c>
+      <c r="J26" s="10">
+        <v>8</v>
+      </c>
+      <c r="K26" s="10">
+        <v>9</v>
+      </c>
+      <c r="L26" s="10">
+        <v>10</v>
+      </c>
+      <c r="P26" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="10">
+        <v>2</v>
+      </c>
+      <c r="R26" s="10">
+        <v>3</v>
+      </c>
+      <c r="S26" s="10">
+        <v>4</v>
+      </c>
+      <c r="T26" s="10">
+        <v>5</v>
+      </c>
+      <c r="U26" s="10">
+        <v>6</v>
+      </c>
+      <c r="V26" s="10">
+        <v>7</v>
+      </c>
+      <c r="W26" s="10">
+        <v>8</v>
+      </c>
+      <c r="X26" s="10">
+        <v>9</v>
+      </c>
+      <c r="Y26" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B27" s="10">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="O27" s="10">
+        <v>1</v>
+      </c>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="11"/>
+      <c r="Y27" s="11"/>
+    </row>
+    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B28" s="10">
+        <v>2</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="O28" s="10">
+        <v>2</v>
+      </c>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+      <c r="X28" s="11"/>
+      <c r="Y28" s="11"/>
+    </row>
+    <row r="29" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B29" s="10">
+        <v>3</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="O29" s="10">
+        <v>3</v>
+      </c>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="W29" s="11"/>
+      <c r="X29" s="11"/>
+      <c r="Y29" s="11"/>
+    </row>
+    <row r="30" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B30" s="10">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="O30" s="10">
+        <v>4</v>
+      </c>
+      <c r="P30" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+    </row>
+    <row r="31" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B31" s="10">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="O31" s="10">
+        <v>5</v>
+      </c>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7"/>
+    </row>
+    <row r="32" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B32" s="10">
+        <v>6</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="O32" s="10">
+        <v>6</v>
+      </c>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
+      <c r="Y32" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B33" s="10">
+        <v>7</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="O33" s="10">
+        <v>7</v>
+      </c>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+    </row>
+    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B34" s="10">
+        <v>8</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="O34" s="10">
+        <v>8</v>
+      </c>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+    </row>
+    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B35" s="10">
+        <v>9</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="O35" s="10">
+        <v>9</v>
+      </c>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="6"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1"/>
+    </row>
+    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B36" s="10">
+        <v>10</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="O36" s="10">
+        <v>10</v>
+      </c>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>